<commit_message>
actualiza trasparencia, 2 boletines y 41 solicitudes de información
</commit_message>
<xml_diff>
--- a/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1677F577-FA45-4674-9592-E7199EFB5EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01E97F92-DCD8-4A18-A550-809B611FE356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
@@ -304,13 +304,13 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  abril 2022</t>
+    <t>Fecha de Actualización y/o Revisión:MAYO 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: abril 2022</t>
+    <t>Fecha de Actualización y/o Revisión: MAYO 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:abril 2022</t>
+    <t>Fecha de Actualización y/o Revisión:  MAYO 2022</t>
   </si>
 </sst>
 </file>
@@ -773,6 +773,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -788,11 +791,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -823,9 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1175,25 +1175,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -1206,25 +1206,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -1237,32 +1237,32 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49" t="s">
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="50" t="s">
         <v>7</v>
       </c>
@@ -1280,37 +1280,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49" t="s">
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="44" t="s">
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="Q4" s="45" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -1325,13 +1325,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1353,9 +1353,9 @@
       <c r="N5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -30433,6 +30433,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
@@ -30449,7 +30450,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:K4"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30490,25 +30490,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -30521,25 +30521,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30552,37 +30552,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30595,37 +30595,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30640,13 +30640,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30668,9 +30668,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -32401,6 +32401,7 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -32417,7 +32418,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32458,25 +32458,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -32489,25 +32489,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32520,37 +32520,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32563,37 +32563,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32608,13 +32608,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32636,9 +32636,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34011,6 +34011,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -34027,7 +34028,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34067,25 +34067,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -34098,25 +34098,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34129,37 +34129,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34172,37 +34172,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34217,13 +34217,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34245,9 +34245,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35608,6 +35608,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -35624,7 +35625,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35665,25 +35665,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -35696,25 +35696,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35727,37 +35727,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35770,37 +35770,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35815,13 +35815,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35843,9 +35843,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37324,6 +37324,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -37340,7 +37341,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37380,25 +37380,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
+      <c r="A1" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -37411,25 +37411,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37442,37 +37442,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="57" t="s">
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37485,11 +37485,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="58" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="59" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="62" t="s">
@@ -37498,24 +37498,24 @@
       <c r="G4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61" t="s">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="61" t="s">
+      <c r="P4" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37530,11 +37530,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="62"/>
       <c r="G5" s="62"/>
       <c r="H5" s="15" t="s">
@@ -37558,9 +37558,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39195,6 +39195,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
@@ -39211,7 +39212,6 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se suben cambios de cpc y cc
</commit_message>
<xml_diff>
--- a/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
+++ b/secretaria-ejecutiva/transparencia/art-21-23-catalogos-documentales-de-archivos/catalogo-de-disposicion-gubernamental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E745939E-F469-44A9-98FD-02FCFECAF865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77DBD87A-8193-43D8-8DDC-954D71DBE992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{C57AC4B7-AFE0-460F-B1DE-63E8DE9C1FE7}"/>
   </bookViews>
@@ -304,10 +304,10 @@
     <t>1.2.13 RESPALDO</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión: octubre 2022</t>
+    <t>Fecha de Actualización y/o Revisión: NOVIEMBRE 2022</t>
   </si>
   <si>
-    <t>Fecha de Actualización y/o Revisión:  octubre 2022</t>
+    <t>Fecha de Actualización y/o Revisión:  NOVIEMBRE 2022</t>
   </si>
 </sst>
 </file>
@@ -788,6 +788,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,9 +819,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -30427,6 +30427,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
@@ -30443,7 +30444,6 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -30515,25 +30515,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -30546,37 +30546,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -30589,37 +30589,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="56" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59" t="s">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="50" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -30634,13 +30634,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -30662,9 +30662,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="50"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -32395,6 +32395,7 @@
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -32411,7 +32412,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
@@ -32483,25 +32483,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -32514,37 +32514,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -32557,37 +32557,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="56" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59" t="s">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="50" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -32602,13 +32602,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -32630,9 +32630,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="50"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -34005,6 +34005,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -34021,7 +34022,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -34092,25 +34092,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -34123,37 +34123,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -34166,37 +34166,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="56" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59" t="s">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="50" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -34211,13 +34211,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -34239,9 +34239,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="50"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -35602,6 +35602,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:A5"/>
@@ -35618,7 +35619,6 @@
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="52" orientation="landscape" r:id="rId1"/>
@@ -35690,25 +35690,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -35721,37 +35721,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -35764,37 +35764,37 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="56" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59" t="s">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="50" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -35809,13 +35809,13 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
@@ -35837,9 +35837,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="50"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -37318,6 +37318,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -37334,7 +37335,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
@@ -37405,25 +37405,25 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -37436,37 +37436,37 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="55" t="s">
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -37479,11 +37479,11 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="56" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="57" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="61" t="s">
@@ -37492,24 +37492,24 @@
       <c r="G4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="59" t="s">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="50" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="1"/>
@@ -37524,11 +37524,11 @@
       <c r="AA4" s="1"/>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="61"/>
       <c r="G5" s="61"/>
       <c r="H5" s="15" t="s">
@@ -37552,9 +37552,9 @@
       <c r="N5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="50"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -39189,6 +39189,7 @@
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
@@ -39205,7 +39206,6 @@
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>

</xml_diff>